<commit_message>
ADAE MSK update & usage stats update.
</commit_message>
<xml_diff>
--- a/static/fields/animalandveterinaryevent_reference.xlsx
+++ b/static/fields/animalandveterinaryevent_reference.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackfinch/WebstormProjects/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8571973-B763-0441-80D7-2C371015B6F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F5D0CA-6345-604C-BBDB-42396DD6E657}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="28240" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="drug_event_fields" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" iterateDelta="1E-4"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="164">
   <si>
     <t>Field Name</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>For the purposes of OpenFDA, this number represents a unique report identification number documented in the FDA CVM database.</t>
+  </si>
+  <si>
+    <t>Note: MSK is a null flavor that means "masked." MSK is used when there is information available for the value, but it has not been provided to the sender due to security, privacy, or other reasons.</t>
   </si>
 </sst>
 </file>
@@ -677,7 +680,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -699,6 +702,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="99">
@@ -1140,72 +1146,66 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="118.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79" style="5" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1213,13 +1213,13 @@
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1227,13 +1227,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1241,41 +1241,41 @@
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1283,27 +1283,27 @@
         <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1311,13 +1311,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1325,13 +1325,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1339,13 +1339,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1353,27 +1353,27 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1381,13 +1381,13 @@
         <v>41</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1395,13 +1395,13 @@
         <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1409,80 +1409,80 @@
         <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="C20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -1490,13 +1490,13 @@
         <v>46</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -1504,27 +1504,27 @@
         <v>46</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1532,13 +1532,13 @@
         <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1546,13 +1546,13 @@
         <v>46</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1560,27 +1560,27 @@
         <v>46</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1588,27 +1588,27 @@
         <v>66</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1616,13 +1616,13 @@
         <v>46</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1630,13 +1630,13 @@
         <v>46</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1644,52 +1644,52 @@
         <v>46</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>38</v>
+        <v>3</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="5" t="s">
+      <c r="C39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1697,13 +1697,13 @@
         <v>46</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1711,13 +1711,13 @@
         <v>46</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>87</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1725,27 +1725,27 @@
         <v>46</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -1753,27 +1753,27 @@
         <v>46</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1781,52 +1781,52 @@
         <v>46</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1834,38 +1834,38 @@
         <v>101</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="5" t="s">
+      <c r="C51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B52" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D52" s="5" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1873,160 +1873,160 @@
         <v>105</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D53" s="5" t="s">
+      <c r="C54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B55" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>87</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B59" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D59" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D61" s="5" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B61" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B63" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D63" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2034,13 +2034,13 @@
         <v>125</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2048,38 +2048,38 @@
         <v>125</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D68" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B69" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D69" s="5" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2087,13 +2087,13 @@
         <v>135</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2101,13 +2101,13 @@
         <v>135</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2115,13 +2115,13 @@
         <v>135</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2129,13 +2129,13 @@
         <v>135</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2143,95 +2143,110 @@
         <v>135</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D74" s="5" t="s">
+      <c r="C75" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="B76" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D75" s="5" t="s">
+      <c r="C76" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B77" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D76" s="5" t="s">
+      <c r="C77" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="5" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B77" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B79" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B80" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B82" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C81" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D81" s="5" t="s">
+      <c r="C82" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="87" spans="2:4" ht="48" x14ac:dyDescent="0.2"/>
-    <row r="88" spans="2:4" ht="32" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="21" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>